<commit_message>
All input cells pass
Formulas are bucketed as anything with an =, it appears
</commit_message>
<xml_diff>
--- a/src/test/resources/small-worksheet.xlsx
+++ b/src/test/resources/small-worksheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KevinLubick\Documents\GitHub\spreadsheet-analyzer\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KevinLubick\Downloads\Source\xlAnalysis\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -74,8 +74,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -359,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:P17"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -370,19 +371,31 @@
     <col min="14" max="14" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16">
-      <c r="C3" s="1" t="s">
+    <row r="1" spans="1:16">
+      <c r="A1" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
       <c r="M3" t="s">
         <v>1</v>
       </c>
@@ -393,7 +406,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:16">
+    <row r="4" spans="1:16">
       <c r="C4">
         <v>1</v>
       </c>
@@ -432,7 +445,7 @@
         <v>43.58591579635798</v>
       </c>
     </row>
-    <row r="5" spans="2:16">
+    <row r="5" spans="1:16">
       <c r="B5">
         <v>1</v>
       </c>
@@ -484,11 +497,11 @@
         <v>3</v>
       </c>
       <c r="P5">
-        <f t="shared" ref="P5:P17" si="2">LOG(MAX($C$5:$M$17),O5)</f>
+        <f t="shared" ref="P5:P16" si="2">LOG(MAX($C$5:$M$17),O5)</f>
         <v>27.499651112582431</v>
       </c>
     </row>
-    <row r="6" spans="2:16">
+    <row r="6" spans="1:16">
       <c r="B6">
         <v>2</v>
       </c>
@@ -547,7 +560,7 @@
         <v>21.79295789817899</v>
       </c>
     </row>
-    <row r="7" spans="2:16">
+    <row r="7" spans="1:16">
       <c r="B7">
         <v>3</v>
       </c>
@@ -597,7 +610,7 @@
       </c>
       <c r="N7">
         <f>COUNT(A1:M20)</f>
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="O7">
         <v>5</v>
@@ -607,7 +620,7 @@
         <v>18.771432195652185</v>
       </c>
     </row>
-    <row r="8" spans="2:16">
+    <row r="8" spans="1:16">
       <c r="B8">
         <v>4</v>
       </c>
@@ -663,7 +676,7 @@
         <v>16.861333881709434</v>
       </c>
     </row>
-    <row r="9" spans="2:16">
+    <row r="9" spans="1:16">
       <c r="B9">
         <v>5</v>
       </c>
@@ -719,7 +732,7 @@
         <v>15.525616463347786</v>
       </c>
     </row>
-    <row r="10" spans="2:16">
+    <row r="10" spans="1:16">
       <c r="B10">
         <v>6</v>
       </c>
@@ -775,7 +788,7 @@
         <v>14.528638598785994</v>
       </c>
     </row>
-    <row r="11" spans="2:16">
+    <row r="11" spans="1:16">
       <c r="B11">
         <v>7</v>
       </c>
@@ -831,7 +844,7 @@
         <v>13.749825556291215</v>
       </c>
     </row>
-    <row r="12" spans="2:16">
+    <row r="12" spans="1:16">
       <c r="B12">
         <v>8</v>
       </c>
@@ -887,7 +900,7 @@
         <v>13.12066804318829</v>
       </c>
     </row>
-    <row r="13" spans="2:16">
+    <row r="13" spans="1:16">
       <c r="B13">
         <v>9</v>
       </c>
@@ -943,7 +956,7 @@
         <v>12.599155179580302</v>
       </c>
     </row>
-    <row r="14" spans="2:16">
+    <row r="14" spans="1:16">
       <c r="B14">
         <v>10</v>
       </c>
@@ -999,7 +1012,7 @@
         <v>12.157983741138205</v>
       </c>
     </row>
-    <row r="15" spans="2:16">
+    <row r="15" spans="1:16">
       <c r="B15">
         <v>11</v>
       </c>
@@ -1055,7 +1068,7 @@
         <v>11.778577443832342</v>
       </c>
     </row>
-    <row r="16" spans="2:16">
+    <row r="16" spans="1:16">
       <c r="B16">
         <v>12</v>
       </c>
@@ -1158,6 +1171,14 @@
       <c r="M17">
         <f t="shared" si="1"/>
         <v>13202860761145</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13">
+      <c r="G19">
+        <v>3.1415000000000002</v>
+      </c>
+      <c r="L19" s="1">
+        <v>42077</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first crack at references
</commit_message>
<xml_diff>
--- a/src/test/resources/small-worksheet.xlsx
+++ b/src/test/resources/small-worksheet.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9750"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9750" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -362,8 +363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -454,11 +455,11 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <f>POWER(D$4,$B5)</f>
+        <f t="shared" ref="D5:I5" si="0">POWER(D$4,$B5)</f>
         <v>2</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:L17" si="0">POWER(E$4,$B5)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="F5">
@@ -478,26 +479,26 @@
         <v>7</v>
       </c>
       <c r="J5">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E5:L17" si="1">POWER(J$4,$B5)</f>
         <v>8</v>
       </c>
       <c r="K5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="L5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="M5">
-        <f t="shared" ref="M5:M17" si="1">SUM(C5:L5)</f>
+        <f t="shared" ref="M5:M17" si="2">SUM(C5:L5)</f>
         <v>55</v>
       </c>
       <c r="O5">
         <v>3</v>
       </c>
       <c r="P5">
-        <f t="shared" ref="P5:P16" si="2">LOG(MAX($C$5:$M$17),O5)</f>
+        <f t="shared" ref="P5:P16" si="3">LOG(MAX($C$5:$M$17),O5)</f>
         <v>27.499651112582431</v>
       </c>
     </row>
@@ -506,47 +507,47 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <f t="shared" ref="C6:D17" si="3">POWER(C$4,$B6)</f>
+        <f t="shared" ref="C6:D17" si="4">POWER(C$4,$B6)</f>
         <v>1</v>
       </c>
       <c r="D6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="I6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="J6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>64</v>
       </c>
       <c r="K6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>81</v>
       </c>
       <c r="L6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="M6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>385</v>
       </c>
       <c r="N6" t="s">
@@ -556,7 +557,7 @@
         <v>4</v>
       </c>
       <c r="P6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21.79295789817899</v>
       </c>
     </row>
@@ -565,47 +566,47 @@
         <v>3</v>
       </c>
       <c r="C7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="D7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>64</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>125</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>216</v>
       </c>
       <c r="I7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>343</v>
       </c>
       <c r="J7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>512</v>
       </c>
       <c r="K7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>729</v>
       </c>
       <c r="L7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="M7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3025</v>
       </c>
       <c r="N7">
@@ -616,7 +617,7 @@
         <v>5</v>
       </c>
       <c r="P7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18.771432195652185</v>
       </c>
     </row>
@@ -625,54 +626,54 @@
         <v>4</v>
       </c>
       <c r="C8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="D8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>81</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>256</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>625</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1296</v>
       </c>
       <c r="I8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2401</v>
       </c>
       <c r="J8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4096</v>
       </c>
       <c r="K8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6561</v>
       </c>
       <c r="L8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10000</v>
       </c>
       <c r="M8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25333</v>
       </c>
       <c r="O8">
         <v>6</v>
       </c>
       <c r="P8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16.861333881709434</v>
       </c>
     </row>
@@ -681,54 +682,54 @@
         <v>5</v>
       </c>
       <c r="C9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="D9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>243</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1024</v>
       </c>
       <c r="G9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3125</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7776</v>
       </c>
       <c r="I9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16807</v>
       </c>
       <c r="J9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32768</v>
       </c>
       <c r="K9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>59049</v>
       </c>
       <c r="L9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>100000</v>
       </c>
       <c r="M9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>220825</v>
       </c>
       <c r="O9">
         <v>7</v>
       </c>
       <c r="P9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.525616463347786</v>
       </c>
     </row>
@@ -737,54 +738,54 @@
         <v>6</v>
       </c>
       <c r="C10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="D10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>64</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>729</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4096</v>
       </c>
       <c r="G10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15625</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46656</v>
       </c>
       <c r="I10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>117649</v>
       </c>
       <c r="J10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>262144</v>
       </c>
       <c r="K10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>531441</v>
       </c>
       <c r="L10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1000000</v>
       </c>
       <c r="M10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1978405</v>
       </c>
       <c r="O10">
         <v>8</v>
       </c>
       <c r="P10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14.528638598785994</v>
       </c>
     </row>
@@ -793,54 +794,54 @@
         <v>7</v>
       </c>
       <c r="C11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="D11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>128</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2187</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16384</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>78125</v>
       </c>
       <c r="H11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>279936</v>
       </c>
       <c r="I11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>823543</v>
       </c>
       <c r="J11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2097152</v>
       </c>
       <c r="K11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4782969</v>
       </c>
       <c r="L11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10000000</v>
       </c>
       <c r="M11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18080425</v>
       </c>
       <c r="O11">
         <v>9</v>
       </c>
       <c r="P11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13.749825556291215</v>
       </c>
     </row>
@@ -849,54 +850,54 @@
         <v>8</v>
       </c>
       <c r="C12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="D12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>256</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6561</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>65536</v>
       </c>
       <c r="G12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>390625</v>
       </c>
       <c r="H12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1679616</v>
       </c>
       <c r="I12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5764801</v>
       </c>
       <c r="J12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16777216</v>
       </c>
       <c r="K12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43046721</v>
       </c>
       <c r="L12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>100000000</v>
       </c>
       <c r="M12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>167731333</v>
       </c>
       <c r="O12">
         <v>10</v>
       </c>
       <c r="P12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13.12066804318829</v>
       </c>
     </row>
@@ -905,54 +906,54 @@
         <v>9</v>
       </c>
       <c r="C13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="D13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>512</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19683</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>262144</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1953125</v>
       </c>
       <c r="H13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10077696</v>
       </c>
       <c r="I13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40353607</v>
       </c>
       <c r="J13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>134217728</v>
       </c>
       <c r="K13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>387420489</v>
       </c>
       <c r="L13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1000000000</v>
       </c>
       <c r="M13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1574304985</v>
       </c>
       <c r="O13">
         <v>11</v>
       </c>
       <c r="P13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12.599155179580302</v>
       </c>
     </row>
@@ -961,54 +962,54 @@
         <v>10</v>
       </c>
       <c r="C14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="D14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1024</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>59049</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1048576</v>
       </c>
       <c r="G14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9765625</v>
       </c>
       <c r="H14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>60466176</v>
       </c>
       <c r="I14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>282475249</v>
       </c>
       <c r="J14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1073741824</v>
       </c>
       <c r="K14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3486784401</v>
       </c>
       <c r="L14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10000000000</v>
       </c>
       <c r="M14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14914341925</v>
       </c>
       <c r="O14">
         <v>12</v>
       </c>
       <c r="P14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12.157983741138205</v>
       </c>
     </row>
@@ -1017,54 +1018,54 @@
         <v>11</v>
       </c>
       <c r="C15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="D15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2048</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>177147</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4194304</v>
       </c>
       <c r="G15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48828125</v>
       </c>
       <c r="H15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>362797056</v>
       </c>
       <c r="I15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1977326743</v>
       </c>
       <c r="J15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8589934592</v>
       </c>
       <c r="K15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>31381059609</v>
       </c>
       <c r="L15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>100000000000</v>
       </c>
       <c r="M15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>142364319625</v>
       </c>
       <c r="O15">
         <v>13</v>
       </c>
       <c r="P15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11.778577443832342</v>
       </c>
     </row>
@@ -1073,54 +1074,54 @@
         <v>12</v>
       </c>
       <c r="C16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="D16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4096</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>531441</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16777216</v>
       </c>
       <c r="G16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>244140625</v>
       </c>
       <c r="H16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2176782336</v>
       </c>
       <c r="I16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13841287201</v>
       </c>
       <c r="J16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>68719476736</v>
       </c>
       <c r="K16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>282429536481</v>
       </c>
       <c r="L16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1000000000000</v>
       </c>
       <c r="M16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1367428536133</v>
       </c>
       <c r="O16">
         <v>14</v>
       </c>
       <c r="P16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11.447820518083693</v>
       </c>
     </row>
@@ -1129,47 +1130,47 @@
         <v>13</v>
       </c>
       <c r="C17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="D17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8192</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1594323</v>
       </c>
       <c r="F17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>67108864</v>
       </c>
       <c r="G17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1220703125</v>
       </c>
       <c r="H17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13060694016</v>
       </c>
       <c r="I17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>96889010407</v>
       </c>
       <c r="J17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>549755813888</v>
       </c>
       <c r="K17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2541865828329</v>
       </c>
       <c r="L17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10000000000000</v>
       </c>
       <c r="M17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13202860761145</v>
       </c>
     </row>
@@ -1187,4 +1188,29 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E6:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="6" spans="5:7">
+      <c r="E6" s="1">
+        <f>1+Sheet1!L19</f>
+        <v>42078</v>
+      </c>
+      <c r="G6">
+        <f>COUNT(Sheet1!O1:P24)</f>
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Completes referenced input cells
</commit_message>
<xml_diff>
--- a/src/test/resources/small-worksheet.xlsx
+++ b/src/test/resources/small-worksheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9750" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9750"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,6 +46,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -75,12 +78,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -361,10 +365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -610,7 +614,7 @@
         <v>3025</v>
       </c>
       <c r="N7">
-        <f>COUNT(A1:M20)</f>
+        <f>COUNT(A4:M20)</f>
         <v>168</v>
       </c>
       <c r="O7">
@@ -1180,6 +1184,11 @@
       </c>
       <c r="L19" s="1">
         <v>42077</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13">
+      <c r="C23" s="3">
+        <v>1234.56</v>
       </c>
     </row>
   </sheetData>
@@ -1187,6 +1196,7 @@
     <mergeCell ref="C3:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1194,8 +1204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E6:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>

<commit_message>
Add tests for function eval type
</commit_message>
<xml_diff>
--- a/src/test/resources/small-worksheet.xlsx
+++ b/src/test/resources/small-worksheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KevinLubick\Downloads\Source\xlAnalysis\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -49,7 +49,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,10 +81,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -368,15 +368,15 @@
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="14" max="14" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -387,20 +387,24 @@
       <c r="E1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="C3" s="2" t="s">
+      <c r="F1" t="b">
+        <f>AND(D1,E1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
       <c r="M3" t="s">
         <v>1</v>
       </c>
@@ -411,7 +415,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>1</v>
       </c>
@@ -450,7 +454,7 @@
         <v>43.58591579635798</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1</v>
       </c>
@@ -506,7 +510,7 @@
         <v>27.499651112582431</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>2</v>
       </c>
@@ -565,7 +569,7 @@
         <v>21.79295789817899</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>3</v>
       </c>
@@ -625,7 +629,7 @@
         <v>18.771432195652185</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>4</v>
       </c>
@@ -681,7 +685,7 @@
         <v>16.861333881709434</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>5</v>
       </c>
@@ -737,7 +741,7 @@
         <v>15.525616463347786</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>6</v>
       </c>
@@ -793,7 +797,7 @@
         <v>14.528638598785994</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>7</v>
       </c>
@@ -849,7 +853,7 @@
         <v>13.749825556291215</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>8</v>
       </c>
@@ -905,7 +909,7 @@
         <v>13.12066804318829</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>9</v>
       </c>
@@ -961,7 +965,7 @@
         <v>12.599155179580302</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>10</v>
       </c>
@@ -1017,7 +1021,7 @@
         <v>12.157983741138205</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>11</v>
       </c>
@@ -1073,7 +1077,7 @@
         <v>11.778577443832342</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>12</v>
       </c>
@@ -1129,7 +1133,7 @@
         <v>11.447820518083693</v>
       </c>
     </row>
-    <row r="17" spans="2:13">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>13</v>
       </c>
@@ -1178,7 +1182,7 @@
         <v>13202860761145</v>
       </c>
     </row>
-    <row r="19" spans="2:13">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="G19">
         <v>3.1415000000000002</v>
       </c>
@@ -1186,8 +1190,8 @@
         <v>42077</v>
       </c>
     </row>
-    <row r="23" spans="2:13">
-      <c r="C23" s="3">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C23" s="2">
         <v>1234.56</v>
       </c>
     </row>
@@ -1208,9 +1212,9 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="6" spans="5:7">
+    <row r="6" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E6" s="1">
         <f>1+Sheet1!L19</f>
         <v>42078</v>

</xml_diff>

<commit_message>
Add test for contains macros xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/small-worksheet.xlsx
+++ b/src/test/resources/small-worksheet.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420" codeName="{7A2D7E96-6E34-419A-AE5F-296B3A7E7977}"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\"/>
@@ -100,6 +100,70 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>66675</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>15</xdr:col>
+          <xdr:colOff>57150</xdr:colOff>
+          <xdr:row>23</xdr:row>
+          <xdr:rowOff>142875</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="CommandButton21" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -364,11 +428,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,11 +1266,41 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <controls>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1025" r:id="rId4" name="CommandButton21">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>276225</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>15</xdr:col>
+                <xdr:colOff>57150</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1025" r:id="rId4" name="CommandButton21"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </controls>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="E6:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>